<commit_message>
agregue los archivos de pruebas
</commit_message>
<xml_diff>
--- a/pruebas/pantalla ciudad.xlsx
+++ b/pruebas/pantalla ciudad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Blueweb\Proyectos\Aplicacion77\pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erick Chavarria\Desktop\PruebasCesar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99B625E-B674-44CD-A3BA-7020E586006A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3BDD93-176A-4424-BA10-D0440AA95BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t xml:space="preserve">No </t>
   </si>
@@ -46,12 +46,6 @@
     <t>Funcionalidad</t>
   </si>
   <si>
-    <t>Proyecto</t>
-  </si>
-  <si>
-    <t>Pantalla</t>
-  </si>
-  <si>
     <t>Revision de Formularios</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
     <t>Consulta datos grafica</t>
   </si>
   <si>
-    <t>grafica con datos mostrados con exito.</t>
-  </si>
-  <si>
     <t>Pantalla Ciudad</t>
   </si>
   <si>
@@ -154,27 +145,12 @@
     <t>Boton de agregar</t>
   </si>
   <si>
-    <t>agrega registos a la tabla al llenar los campos solicitados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elementos eliminados con exito </t>
-  </si>
-  <si>
-    <t>elementos agregados con éxito</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boton de modificar </t>
   </si>
   <si>
     <t>que cada registro se modifique en la tabla</t>
   </si>
   <si>
-    <t>modifica los campos de la tabla</t>
-  </si>
-  <si>
-    <t>elementos modificados exitosamente</t>
-  </si>
-  <si>
     <t xml:space="preserve">que la tabla represente los datos obtenidos de la base de datos de la tabla ciudades. </t>
   </si>
   <si>
@@ -184,28 +160,61 @@
     <t xml:space="preserve">que la tabla agregue un nuevo registro  la tabla </t>
   </si>
   <si>
-    <t>editar solo un dato de la fila</t>
-  </si>
-  <si>
     <t>se intenta editar solo un campo</t>
   </si>
   <si>
-    <t>edita un campo y manda ese valor a la funcion de editar, ignorando los otros</t>
-  </si>
-  <si>
-    <t>edita un solo campo dejando los otros iguales</t>
-  </si>
-  <si>
     <t>Editar 2 datos de la fila</t>
   </si>
   <si>
-    <t>edita 2 campos del registro dejando el tercero igual</t>
-  </si>
-  <si>
-    <t>edita solo los 2 campos exitosamente</t>
-  </si>
-  <si>
     <t>se intenta editar 2 campos sin que cambie el tercero</t>
+  </si>
+  <si>
+    <t>al presionar el boton enter al agregar se enviar el formulario correctamente</t>
+  </si>
+  <si>
+    <t>El boton de agregar, agrega correctamente al presionar enter</t>
+  </si>
+  <si>
+    <t>Proyecto BlueWeb</t>
+  </si>
+  <si>
+    <t>Cuando se abre el modal para eliminar, y se llenan lo campos, al presionar enter se activa el boton de agregar</t>
+  </si>
+  <si>
+    <t>Edita 2 campos del registro dejando el tercero igual</t>
+  </si>
+  <si>
+    <t>Edita un campo y manda ese valor a la funcion de editar, ignorando los otros</t>
+  </si>
+  <si>
+    <t>Modifica los campos de la tabla</t>
+  </si>
+  <si>
+    <t>Agrega registos a la tabla al llenar los campos solicitados</t>
+  </si>
+  <si>
+    <t>Editar solo un dato de la fila</t>
+  </si>
+  <si>
+    <t>Presionar boton enter</t>
+  </si>
+  <si>
+    <t>Grafica con datos mostrados con exito.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementos eliminados con exito </t>
+  </si>
+  <si>
+    <t>Elementos agregados con éxito</t>
+  </si>
+  <si>
+    <t>Elementos modificados exitosamente</t>
+  </si>
+  <si>
+    <t>Edita un solo campo dejando los otros iguales</t>
+  </si>
+  <si>
+    <t>Edita solo los 2 campos exitosamente</t>
   </si>
 </sst>
 </file>
@@ -619,22 +628,22 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="I2" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
@@ -644,28 +653,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -673,28 +682,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -702,28 +711,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -731,26 +740,26 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2"/>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1">
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -758,26 +767,26 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2"/>
       <c r="I7" s="1">
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -785,28 +794,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" s="1">
         <v>6</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -814,28 +823,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1">
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" s="1">
         <v>7</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -843,20 +852,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3"/>
       <c r="I10" s="1">
         <v>8</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -895,7 +904,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +917,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -918,7 +927,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -951,19 +960,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D4" s="7">
         <v>44425</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -971,19 +980,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D5" s="7">
         <v>44425</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,19 +1000,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D6" s="7">
         <v>44425</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,19 +1020,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D7" s="12">
         <v>44425</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,19 +1040,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D8" s="12">
         <v>44427</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,28 +1060,40 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D9" s="12">
         <v>44427</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="12">
+        <v>44431</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>

</xml_diff>